<commit_message>
Huge spell overhaul continues
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/bookNames.xlsx
+++ b/CoreRulebook/Data/Spells/bookNames.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HPRPG\CoreRulebook\Data\Spells\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B152CED2-E48E-454F-93B1-D12BBBD1D8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8382DB69-BB03-4445-AE6C-EB792A7AEF5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="16440" xr2:uid="{57F1FBE5-6DB3-4630-913D-5B96B2F02C01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{57F1FBE5-6DB3-4630-913D-5B96B2F02C01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,9 +131,6 @@
     <t>Spelles Moste Vyle</t>
   </si>
   <si>
-    <t>The Necromnicon</t>
-  </si>
-  <si>
     <t>The Dream Oracle</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>Theories on the World Beyond</t>
+  </si>
+  <si>
+    <t>Secrets of the Darkest Art</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,16 +757,16 @@
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>25</v>
@@ -800,22 +800,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -823,22 +823,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -846,22 +846,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -869,68 +869,68 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -938,22 +938,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="E10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -961,22 +961,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -984,22 +984,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1007,22 +1007,22 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>30</v>
@@ -1045,7 +1045,7 @@
         <v>31</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1056,19 +1056,19 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>